<commit_message>
change in email name
</commit_message>
<xml_diff>
--- a/MyStoreProjectDataDriven/src/test/resources/TestData/TestData.xlsx
+++ b/MyStoreProjectDataDriven/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>ghfsdtyfg@gmail.com</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>Test1234</t>
+  </si>
+  <si>
+    <t>gfsdtyfg@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1046,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1066,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" activeCellId="1" sqref="A1 A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1080,7 +1082,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1096,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1184,187 +1186,187 @@
         <v>50</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="F2" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="F3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="F4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="N4" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="O4" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chnage in excel data
</commit_message>
<xml_diff>
--- a/MyStoreProjectDataDriven/src/test/resources/TestData/TestData.xlsx
+++ b/MyStoreProjectDataDriven/src/test/resources/TestData/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
   <si>
     <t>TestCases</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>hgsdtyf</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
@@ -224,18 +221,9 @@
     <t>1985</t>
   </si>
   <si>
-    <t>TestUser</t>
-  </si>
-  <si>
     <t>UserTest</t>
   </si>
   <si>
-    <t>newtest2@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest3@gmail.com</t>
-  </si>
-  <si>
     <t>opeye@gmail.com</t>
   </si>
   <si>
@@ -245,7 +233,22 @@
     <t>gfsdyfg@gmail.com</t>
   </si>
   <si>
-    <t>newtest10@gmail.com</t>
+    <t>newt@gmail.com</t>
+  </si>
+  <si>
+    <t>qas2@gmail.com</t>
+  </si>
+  <si>
+    <t>qad3@gmail.com</t>
+  </si>
+  <si>
+    <t>TestUsee</t>
+  </si>
+  <si>
+    <t>TestUsew</t>
+  </si>
+  <si>
+    <t>TestUsey</t>
   </si>
 </sst>
 </file>
@@ -991,7 +994,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1030,10 +1033,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1111,7 +1114,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,71 +1153,71 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="E4" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>